<commit_message>
Changes and Initial Version
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56535C\Documents\UiPath\P004_SP004_090_NewHireCommunication_NewHirePaperWork_Perfomer\P004_SP004_090_NewHireCommunication_NewHirePaperWork_Perfomer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56535C\Documents\UiPath\P004_SP004_090_NewHireCommunication_NewHirePaperWork_Perfomer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D033159A-0E47-489F-B31B-85D2F8C3B9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DCDAED-1038-4605-A207-639ACC36A9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -159,13 +159,58 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>AdobeSignURL</t>
   </si>
   <si>
     <t>Adobe Sign</t>
+  </si>
+  <si>
+    <t>P004_SP004_090_NHC_NHP_Performer_Queue</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>AdobeSignEmailAddress</t>
+  </si>
+  <si>
+    <t>P004_SP004_090_AdobeSignEmailAddress</t>
+  </si>
+  <si>
+    <t>O365AppID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationID</t>
+  </si>
+  <si>
+    <t>O365TenantID</t>
+  </si>
+  <si>
+    <t>Shared_O365TenantID</t>
+  </si>
+  <si>
+    <t>O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>NHC_SharepointURL</t>
+  </si>
+  <si>
+    <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication</t>
+  </si>
+  <si>
+    <t>NHC_SharepointListName</t>
+  </si>
+  <si>
+    <t>New Hire Employee Details</t>
+  </si>
+  <si>
+    <t>DOH_ColumnDisplayName</t>
+  </si>
+  <si>
+    <t>DateOfHire</t>
   </si>
 </sst>
 </file>
@@ -553,7 +598,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -603,7 +648,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -613,7 +658,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -1635,7 +1682,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A22" sqref="A22:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1818,18 +1865,60 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2807,12 +2896,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.33203125" customWidth="1"/>
     <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
@@ -2853,7 +2944,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Bug Fixes and Latest Workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56535C\Documents\UiPath\P004_SP004_090_NewHireCommunication_NewHirePaperWork_Perfomer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DCDAED-1038-4605-A207-639ACC36A9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4626D9-EF9E-4ECB-A571-3DEC9D79CA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -162,9 +162,6 @@
     <t>AdobeSignURL</t>
   </si>
   <si>
-    <t>Adobe Sign</t>
-  </si>
-  <si>
     <t>P004_SP004_090_NHC_NHP_Performer_Queue</t>
   </si>
   <si>
@@ -211,6 +208,36 @@
   </si>
   <si>
     <t>DateOfHire</t>
+  </si>
+  <si>
+    <t>https://omesofm.na1.documents.adobe.com/account/homeJS</t>
+  </si>
+  <si>
+    <t>FillingFieldURL</t>
+  </si>
+  <si>
+    <t>https://omesofm.na1.documents.adobe.com/account</t>
+  </si>
+  <si>
+    <t>MinimumDelay</t>
+  </si>
+  <si>
+    <t>Sharepoint URL</t>
+  </si>
+  <si>
+    <t>https://officemgmtentserv.sharepoint.com/sites/ACOE_Automations_DEV</t>
+  </si>
+  <si>
+    <t>Root Folder</t>
+  </si>
+  <si>
+    <t>P003_090_TimesheetApprovals</t>
+  </si>
+  <si>
+    <t>LocalDownloadPath</t>
+  </si>
+  <si>
+    <t>Data\Input</t>
   </si>
 </sst>
 </file>
@@ -648,7 +675,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -659,7 +686,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
@@ -1681,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1868,62 +1895,97 @@
         <v>44</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
         <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
         <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
         <v>56</v>
-      </c>
-      <c r="B22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
         <v>58</v>
-      </c>
-      <c r="B23" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
         <v>60</v>
       </c>
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2886,7 +2948,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" display="https://omesofm.na1.documents.adobe.com/account/homeJS" xr:uid="{34760AC8-4C7C-431C-94B0-F02DA6E88E83}"/>
+    <hyperlink ref="B27" r:id="rId1" xr:uid="{34AB2DBC-FC06-47D4-B1F9-046E5642CF21}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2946,10 +3008,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Code Review Push 1
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56535C\Documents\UiPath\P004_SP004_090_NewHireCommunication_NewHirePaperWork_Perfomer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C925EB4-DDC3-4771-B723-878C8E1E1416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6A2E40-5474-4D26-A26C-D98B259FFA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="3336" windowWidth="17280" windowHeight="9024" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -404,6 +404,18 @@
   </si>
   <si>
     <t>P004_SP004_090_Status_ColumnDisplayName</t>
+  </si>
+  <si>
+    <t>LoginRetryScopeError</t>
+  </si>
+  <si>
+    <t>Error in log into Adobe Sign portal</t>
+  </si>
+  <si>
+    <t>WorkflowExperience</t>
+  </si>
+  <si>
+    <t>Try the Modern Experience</t>
   </si>
 </sst>
 </file>
@@ -1877,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2227,8 +2239,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3186,7 +3212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Latest Code Review Code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56535C\Documents\UiPath\P004_SP004_090_NewHireCommunication_NewHirePaperWork_Perfomer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF70E93-A75B-47E7-9A8F-C629B826176E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688AA64B-04FF-4E22-9128-0C40EFBE194A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -186,9 +186,6 @@
     <t>NHC_SharepointListName</t>
   </si>
   <si>
-    <t>https://omesofm.na1.documents.adobe.com/account/homeJS</t>
-  </si>
-  <si>
     <t>FillingFieldURL</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
   </si>
   <si>
     <t>SystemException_EmailSubject</t>
-  </si>
-  <si>
-    <t>The Automation &lt;ProcessName&gt; encountered a system exception.</t>
   </si>
   <si>
     <t>SystemException_EmailBody</t>
@@ -428,6 +422,9 @@
   </si>
   <si>
     <t>P004_SP004_090_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_SP004_090_AdobeSignURL</t>
   </si>
 </sst>
 </file>
@@ -891,7 +888,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -1899,10 +1896,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z981"/>
+  <dimension ref="A1:Z979"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A26"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2085,122 +2082,122 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="5" t="s">
         <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
         <v>55</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
         <v>56</v>
       </c>
-      <c r="B20">
-        <v>2</v>
+      <c r="B20" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="5" t="s">
         <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
+      <c r="A24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="4" t="s">
         <v>71</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" t="s">
-        <v>76</v>
+        <v>101</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>74</v>
+        <v>102</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
@@ -2208,7 +2205,7 @@
         <v>103</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
@@ -2216,7 +2213,7 @@
         <v>104</v>
       </c>
       <c r="B34">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
@@ -2224,7 +2221,7 @@
         <v>105</v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
@@ -2232,41 +2229,27 @@
         <v>106</v>
       </c>
       <c r="B36">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37">
-        <v>0.1</v>
+        <v>117</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A39" t="s">
         <v>119</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B38" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A40" t="s">
-        <v>121</v>
-      </c>
-      <c r="B40" t="s">
-        <v>122</v>
-      </c>
-    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3206,15 +3189,13 @@
     <row r="977" ht="14.25" customHeight="1"/>
     <row r="978" ht="14.25" customHeight="1"/>
     <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B21" r:id="rId1" xr:uid="{34AB2DBC-FC06-47D4-B1F9-046E5642CF21}"/>
-    <hyperlink ref="B30" r:id="rId2" xr:uid="{B11F4239-3559-49C4-94E9-67B8B03D4491}"/>
-    <hyperlink ref="B29" r:id="rId3" xr:uid="{5B7116D6-05B4-4D20-B849-004D66D1F449}"/>
-    <hyperlink ref="B32" r:id="rId4" xr:uid="{9455ED66-F96E-48DB-A543-FA2CFBFD46D4}"/>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{34AB2DBC-FC06-47D4-B1F9-046E5642CF21}"/>
+    <hyperlink ref="B28" r:id="rId2" xr:uid="{B11F4239-3559-49C4-94E9-67B8B03D4491}"/>
+    <hyperlink ref="B27" r:id="rId3" xr:uid="{5B7116D6-05B4-4D20-B849-004D66D1F449}"/>
+    <hyperlink ref="B30" r:id="rId4" xr:uid="{9455ED66-F96E-48DB-A543-FA2CFBFD46D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3225,7 +3206,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3280,62 +3261,62 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
         <v>85</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3343,10 +3324,10 @@
         <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -3354,10 +3335,10 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -3365,10 +3346,10 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -3376,10 +3357,10 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -3387,167 +3368,177 @@
         <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
         <v>125</v>
       </c>
-      <c r="B26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Adobe Sign LDA Page Exception Handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56535C\Documents\UiPath\P004_SP004_090_NewHireCommunication_NewHirePaperWork_Perfomer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBE8A91-7F74-469B-AEC5-EAAA7949AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A61831C-321E-45B9-A4C8-AEB790994950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="156">
   <si>
     <t>Name</t>
   </si>
@@ -498,6 +498,15 @@
   </si>
   <si>
     <t>Bot Sharepoint URL to get the template</t>
+  </si>
+  <si>
+    <t>AdobeLoginCredentialFolder</t>
+  </si>
+  <si>
+    <t>AdobeLoginCredentialAsset</t>
+  </si>
+  <si>
+    <t>P004_SP004_090_AdobeSignLoginCredentials</t>
   </si>
 </sst>
 </file>
@@ -588,7 +597,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,7 +611,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -929,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1017,8 +1025,22 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3284,8 +3306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3423,10 +3445,10 @@
       <c r="B8" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3437,10 +3459,10 @@
       <c r="B9" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3451,10 +3473,10 @@
       <c r="B10" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3468,7 +3490,7 @@
       <c r="C11" t="s">
         <v>124</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3482,7 +3504,7 @@
       <c r="C12" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3496,7 +3518,7 @@
       <c r="C13" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3510,7 +3532,7 @@
       <c r="C14" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3524,7 +3546,7 @@
       <c r="C15" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3538,7 +3560,7 @@
       <c r="C16" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3552,7 +3574,7 @@
       <c r="C17" t="s">
         <v>125</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3580,7 +3602,7 @@
       <c r="C19" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3594,7 +3616,7 @@
       <c r="C20" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3622,7 +3644,7 @@
       <c r="C22" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3636,7 +3658,7 @@
       <c r="C23" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3664,7 +3686,7 @@
       <c r="C25" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3678,7 +3700,7 @@
       <c r="C26" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3692,7 +3714,7 @@
       <c r="C27" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3706,7 +3728,7 @@
       <c r="C28" t="s">
         <v>125</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3720,7 +3742,7 @@
       <c r="C29" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>